<commit_message>
Update commit of code folder
</commit_message>
<xml_diff>
--- a/output/tables/BF_tables.xlsx
+++ b/output/tables/BF_tables.xlsx
@@ -10,13 +10,20 @@
     <sheet name="FCS_shares" sheetId="2" r:id="rId4"/>
     <sheet name="rCSI_shares" sheetId="3" r:id="rId5"/>
     <sheet name="HHS_shares" sheetId="4" r:id="rId6"/>
+    <sheet name="by_mode_means_wt" sheetId="5" r:id="rId7"/>
+    <sheet name="FCS_shares_wt" sheetId="6" r:id="rId8"/>
+    <sheet name="rCSI_shares_wt" sheetId="7" r:id="rId9"/>
+    <sheet name="HHS_shares_wt" sheetId="8" r:id="rId10"/>
+    <sheet name="Comp_Reg" sheetId="9" r:id="rId11"/>
+    <sheet name="Ind_Means_Ttests" sheetId="10" r:id="rId12"/>
+    <sheet name="Ind_Reg" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="81" uniqueCount="47">
   <si>
     <t>Modality_Type</t>
   </si>
@@ -61,6 +68,102 @@
   </si>
   <si>
     <t>HHS_Moderate</t>
+  </si>
+  <si>
+    <t>wmean_FCS</t>
+  </si>
+  <si>
+    <t>wmean_rCSI</t>
+  </si>
+  <si>
+    <t>wmean_HHS</t>
+  </si>
+  <si>
+    <t>Weights_Note</t>
+  </si>
+  <si>
+    <t>No weights supplied</t>
+  </si>
+  <si>
+    <t>FCS_Poor_wt</t>
+  </si>
+  <si>
+    <t>FCS_Borderline_wt</t>
+  </si>
+  <si>
+    <t>FCS_Acceptable_wt</t>
+  </si>
+  <si>
+    <t>rCSI_Low_wt</t>
+  </si>
+  <si>
+    <t>rCSI_Medium_wt</t>
+  </si>
+  <si>
+    <t>rCSI_High_wt</t>
+  </si>
+  <si>
+    <t>HHS_LittleNo_wt</t>
+  </si>
+  <si>
+    <t>HHS_Moderate_wt</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>FES</t>
+  </si>
+  <si>
+    <t>spec</t>
+  </si>
+  <si>
+    <t>unw</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>varname</t>
+  </si>
+  <si>
+    <t>FCS</t>
+  </si>
+  <si>
+    <t>rCSI</t>
+  </si>
+  <si>
+    <t>HHS</t>
+  </si>
+  <si>
+    <t>mean_f2f</t>
+  </si>
+  <si>
+    <t>sd_f2f</t>
+  </si>
+  <si>
+    <t>mean_ph</t>
+  </si>
+  <si>
+    <t>sd_ph</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>tstat</t>
+  </si>
+  <si>
+    <t>pval</t>
   </si>
 </sst>
 </file>
@@ -167,6 +270,260 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1">
+        <v>26.260869565217391</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10.654008865356445</v>
+      </c>
+      <c r="D2" s="1">
+        <v>27.154071807861328</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9.0768823623657227</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.89320307970046997</v>
+      </c>
+      <c r="G2" s="1">
+        <v>-2.2642102241516113</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.023635245859622955</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9.716049382716049</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10.234962463378906</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6.8596663475036621</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7.8895201683044434</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-2.8563830852508545</v>
+      </c>
+      <c r="G3" s="1">
+        <v>7.7392358779907227</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.3737458165376942e-14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.64680622651637143</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.98473811149597168</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.86849850416183472</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.1241145133972168</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.22169230878353119</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-5.4913010597229004</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4.3374004832230639e-08</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.68673401759858421</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.17143157124519348</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.67190855741500854</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.27878913283348083</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-0.014825445599853992</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.7650237083435059</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.077665738761425018</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.89320305499850972</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.37652009725570679</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.3722586631774902</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.017745064571499825</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-2.8563830431674009</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.34249690175056458</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-8.3398799896240234</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.1376658333250118e-16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.22169230145222399</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.041956011205911636</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.2839221954345703</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.3588523017915577e-07</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-0.014825445165428001</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.0095932111144065857</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-1.54541015625</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.12235695868730545</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2882</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
@@ -318,4 +675,281 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1863</v>
+      </c>
+      <c r="C2" s="1">
+        <v>27.154072620215899</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6.8596663395485766</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.86849852796859661</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1019</v>
+      </c>
+      <c r="C3" s="1">
+        <v>27.154072620215899</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6.8596663395485766</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.86849852796859661</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>36.500268384326354</v>
+      </c>
+      <c r="C2" s="1">
+        <v>46.913580246913575</v>
+      </c>
+      <c r="D2" s="1">
+        <v>16.586151368760064</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>25.711481844946029</v>
+      </c>
+      <c r="C3" s="1">
+        <v>60.942100098135434</v>
+      </c>
+      <c r="D3" s="1">
+        <v>13.346418056918546</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>37.842190016103061</v>
+      </c>
+      <c r="C2" s="1">
+        <v>19.484702093397747</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42.673107890499196</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>48.184494602551517</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15.014720314033367</v>
+      </c>
+      <c r="D3" s="1">
+        <v>36.800785083415107</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>79.495437466451961</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20.504562533548039</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>69.283611383709527</v>
+      </c>
+      <c r="C3" s="1">
+        <v>30.71638861629048</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.014825445165428001</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.0095932111144065857</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-1.54541015625</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.12235695868730545</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>